<commit_message>
Adding percentage data to Lab 14
</commit_message>
<xml_diff>
--- a/14_aldosterone_and_sodium_escape/14_aldosterone_and_sodium_escape.xlsx
+++ b/14_aldosterone_and_sodium_escape/14_aldosterone_and_sodium_escape.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="33">
   <si>
     <t>First Run</t>
   </si>
@@ -104,12 +104,24 @@
   <si>
     <t>With Sodium Escape</t>
   </si>
+  <si>
+    <t>With Angiotensin</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>Without Angiotensin</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +134,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -199,28 +218,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -230,10 +227,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -254,27 +252,102 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -564,13 +637,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" t="s">
@@ -579,40 +655,40 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="H1" t="s">
         <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="11">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="11">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="11">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="11">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="11">
         <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -635,22 +711,22 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="60.75" thickBot="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>97</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>98</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>99</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>105</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -673,22 +749,22 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="75.75" thickBot="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>0.1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>0.4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>0.9</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -711,22 +787,22 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="75.75" thickBot="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>3.5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>4.7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>6.1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -738,33 +814,33 @@
       <c r="J5" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="1">
         <v>4.8</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="13">
         <v>6.6</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="45.75" thickBot="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>13</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>8</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -776,33 +852,33 @@
       <c r="J6" s="3">
         <v>17</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="1">
         <v>13</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="1">
         <v>8</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="60.75" thickBot="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>292</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>1956</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>1901</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>1743</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -825,22 +901,22 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="45.75" thickBot="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>18</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>20</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>22</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -863,22 +939,22 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="45.75" thickBot="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>144.19999999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>147.1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>147.80000000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>149</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -901,22 +977,22 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="45.75" thickBot="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>4.3</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>3.5</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <v>3.2</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>2.7</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -939,22 +1015,22 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="60.75" thickBot="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>123</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>123</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <v>121</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>122</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -977,22 +1053,22 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="75.75" thickBot="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>17.100000000000001</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
         <v>17.3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
         <v>17.2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>17.5</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="4" t="s">
@@ -1015,22 +1091,22 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="75.75" thickBot="1">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="1">
         <v>9.9</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1">
         <v>9.5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>7.6</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1053,22 +1129,22 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="75.75" thickBot="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>1.8</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <v>2.6</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <v>3.8</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -1091,22 +1167,22 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="75.75" thickBot="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <v>1.3</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <v>3.4</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -1128,23 +1204,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:13" ht="61.5" customHeight="1" thickBot="1">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="1">
         <v>0.5</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="1">
         <v>0.2</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="1">
         <v>0.24</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="1">
         <v>0.35</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -1167,12 +1243,24 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="90.75" thickBot="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1192,23 +1280,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="90.75" thickBot="1">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.38</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="F18" s="3" t="s">
+    <row r="18" spans="1:16" ht="75.75" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -1230,23 +1318,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="75.75" thickBot="1">
-      <c r="A19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0.125</v>
-      </c>
-      <c r="C19" s="3">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>4.7E-2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="F19" s="3" t="s">
+    <row r="19" spans="1:16" ht="45.75" thickBot="1">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2962</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3036</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3121</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3297</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1268,23 +1356,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="45.75" thickBot="1">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2962</v>
-      </c>
-      <c r="C20" s="3">
-        <v>3036</v>
-      </c>
-      <c r="D20" s="3">
-        <v>3121</v>
-      </c>
-      <c r="E20" s="3">
-        <v>3297</v>
-      </c>
-      <c r="F20" s="3" t="s">
+    <row r="20" spans="1:16" ht="30.75" thickBot="1">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H20" s="4" t="s">
@@ -1307,22 +1395,22 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="30.75" thickBot="1">
-      <c r="A21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3">
-        <v>12.8</v>
-      </c>
-      <c r="C21" s="3">
-        <v>13.5</v>
-      </c>
-      <c r="D21" s="3">
-        <v>15</v>
-      </c>
-      <c r="E21" s="3">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -1344,25 +1432,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="30.75" thickBot="1">
-      <c r="A22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>23</v>
-      </c>
+    <row r="22" spans="1:16">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" thickBot="1">
       <c r="A24" s="6"/>
@@ -1370,22 +1446,22 @@
         <v>24</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J24" s="7"/>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -2151,34 +2227,964 @@
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="30.75" thickBot="1">
+      <c r="A49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="11">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1</v>
+      </c>
+      <c r="D49" s="11">
+        <v>3</v>
+      </c>
+      <c r="E49" s="11">
+        <v>10</v>
+      </c>
+      <c r="F49" s="11">
+        <v>17</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I49" s="11">
+        <v>0</v>
+      </c>
+      <c r="J49" s="11">
+        <v>1</v>
+      </c>
+      <c r="K49" s="11">
+        <v>3</v>
+      </c>
+      <c r="L49" s="11">
+        <v>10</v>
+      </c>
+      <c r="M49" s="11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="14">
+        <f>ABS((B3-B26)/B3)</f>
+        <v>4.1237113402062438E-3</v>
+      </c>
+      <c r="C50" s="14">
+        <f t="shared" ref="C50:F50" si="0">ABS((C3-C26)/C3)</f>
+        <v>1.4285714285714344E-2</v>
+      </c>
+      <c r="D50" s="14">
+        <f t="shared" si="0"/>
+        <v>1.7171717171717199E-2</v>
+      </c>
+      <c r="E50" s="14">
+        <f t="shared" si="0"/>
+        <v>4.8571428571428515E-2</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I50" s="14">
+        <f>ABS((I3-I26)/I3)</f>
+        <v>4.1237113402062438E-3</v>
+      </c>
+      <c r="J50" s="14">
+        <f t="shared" ref="J50:M50" si="1">ABS((J3-J26)/J3)</f>
+        <v>1.3265306122448951E-2</v>
+      </c>
+      <c r="K50" s="14">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L50" s="14">
+        <f t="shared" si="1"/>
+        <v>5.9813084112149584E-2</v>
+      </c>
+      <c r="M50" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="14">
+        <f t="shared" ref="B51:F51" si="2">ABS((B4-B27)/B4)</f>
+        <v>10.999999999999998</v>
+      </c>
+      <c r="C51" s="14">
+        <f t="shared" si="2"/>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="D51" s="14">
+        <f t="shared" si="2"/>
+        <v>1.5555555555555554</v>
+      </c>
+      <c r="E51" s="14">
+        <f t="shared" si="2"/>
+        <v>1.6874999999999998</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="14">
+        <f t="shared" ref="I51:M51" si="3">ABS((I4-I27)/I4)</f>
+        <v>10.999999999999998</v>
+      </c>
+      <c r="J51" s="14">
+        <f t="shared" si="3"/>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="K51" s="14">
+        <f t="shared" si="3"/>
+        <v>1.5555555555555554</v>
+      </c>
+      <c r="L51" s="14">
+        <f t="shared" si="3"/>
+        <v>1.35</v>
+      </c>
+      <c r="M51" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="14">
+        <f t="shared" ref="B52:F52" si="4">ABS((B5-B28)/B5)</f>
+        <v>0.48571428571428577</v>
+      </c>
+      <c r="C52" s="14">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="D52" s="14">
+        <f t="shared" si="4"/>
+        <v>0.31914893617021273</v>
+      </c>
+      <c r="E52" s="14">
+        <f t="shared" si="4"/>
+        <v>0.36065573770491821</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="14">
+        <f t="shared" ref="I52:M52" si="5">ABS((I5-I28)/I5)</f>
+        <v>0.48571428571428577</v>
+      </c>
+      <c r="J52" s="14">
+        <f t="shared" si="5"/>
+        <v>0.34146341463414648</v>
+      </c>
+      <c r="K52" s="14">
+        <f t="shared" si="5"/>
+        <v>0.3125</v>
+      </c>
+      <c r="L52" s="14">
+        <f t="shared" si="5"/>
+        <v>0.31818181818181812</v>
+      </c>
+      <c r="M52" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="14">
+        <f t="shared" ref="B53:F53" si="6">ABS((B6-B29)/B6)</f>
+        <v>0.11500000000000003</v>
+      </c>
+      <c r="C53" s="14">
+        <f t="shared" si="6"/>
+        <v>0.15625</v>
+      </c>
+      <c r="D53" s="14">
+        <f t="shared" si="6"/>
+        <v>8.4615384615384592E-2</v>
+      </c>
+      <c r="E53" s="14">
+        <f t="shared" si="6"/>
+        <v>3.7499999999999978E-2</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53" s="14">
+        <f t="shared" ref="I53:M53" si="7">ABS((I6-I29)/I6)</f>
+        <v>0.11500000000000003</v>
+      </c>
+      <c r="J53" s="14">
+        <f t="shared" si="7"/>
+        <v>0.10588235294117651</v>
+      </c>
+      <c r="K53" s="14">
+        <f t="shared" si="7"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="L53" s="14">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="M53" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="14">
+        <f t="shared" ref="B54:F54" si="8">ABS((B7-B30)/B7)</f>
+        <v>5.1027397260273895E-2</v>
+      </c>
+      <c r="C54" s="14">
+        <f t="shared" si="8"/>
+        <v>6.7331288343558185E-2</v>
+      </c>
+      <c r="D54" s="14">
+        <f t="shared" si="8"/>
+        <v>6.7069963177275121E-2</v>
+      </c>
+      <c r="E54" s="14">
+        <f t="shared" si="8"/>
+        <v>7.9116465863453861E-2</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="14">
+        <f t="shared" ref="I54:M54" si="9">ABS((I7-I30)/I7)</f>
+        <v>5.1027397260273895E-2</v>
+      </c>
+      <c r="J54" s="14">
+        <f t="shared" si="9"/>
+        <v>6.472690148034721E-2</v>
+      </c>
+      <c r="K54" s="14">
+        <f t="shared" si="9"/>
+        <v>7.3541887592788999E-2</v>
+      </c>
+      <c r="L54" s="14">
+        <f t="shared" si="9"/>
+        <v>9.0599294947121059E-2</v>
+      </c>
+      <c r="M54" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="14">
+        <f t="shared" ref="B55:F55" si="10">ABS((B8-B31)/B8)</f>
+        <v>0.24444444444444435</v>
+      </c>
+      <c r="C55" s="14">
+        <f t="shared" si="10"/>
+        <v>0.13499999999999995</v>
+      </c>
+      <c r="D55" s="14">
+        <f t="shared" si="10"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="E55" s="14">
+        <f t="shared" si="10"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="14">
+        <f t="shared" ref="I55:M55" si="11">ABS((I8-I31)/I8)</f>
+        <v>0.24444444444444435</v>
+      </c>
+      <c r="J55" s="14">
+        <f t="shared" si="11"/>
+        <v>0.13499999999999995</v>
+      </c>
+      <c r="K55" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L55" s="14">
+        <f t="shared" si="11"/>
+        <v>0.15333333333333338</v>
+      </c>
+      <c r="M55" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="14">
+        <f t="shared" ref="B56:F56" si="12">ABS((B9-B32)/B9)</f>
+        <v>4.0915395284327166E-2</v>
+      </c>
+      <c r="C56" s="14">
+        <f t="shared" si="12"/>
+        <v>4.4187627464309993E-2</v>
+      </c>
+      <c r="D56" s="14">
+        <f t="shared" si="12"/>
+        <v>3.5859269282814688E-2</v>
+      </c>
+      <c r="E56" s="14">
+        <f t="shared" si="12"/>
+        <v>1.6107382550335607E-2</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I56" s="14">
+        <f t="shared" ref="I56:M56" si="13">ABS((I9-I32)/I9)</f>
+        <v>4.0915395284327166E-2</v>
+      </c>
+      <c r="J56" s="14">
+        <f t="shared" si="13"/>
+        <v>4.4187627464309993E-2</v>
+      </c>
+      <c r="K56" s="14">
+        <f t="shared" si="13"/>
+        <v>3.651115618661261E-2</v>
+      </c>
+      <c r="L56" s="14">
+        <f t="shared" si="13"/>
+        <v>1.807228915662662E-2</v>
+      </c>
+      <c r="M56" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="14">
+        <f t="shared" ref="B57:F57" si="14">ABS((B10-B33)/B10)</f>
+        <v>2.3255813953488292E-2</v>
+      </c>
+      <c r="C57" s="14">
+        <f t="shared" si="14"/>
+        <v>2.8571428571428598E-2</v>
+      </c>
+      <c r="D57" s="14">
+        <f t="shared" si="14"/>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="E57" s="14">
+        <f t="shared" si="14"/>
+        <v>0.25925925925925913</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I57" s="14">
+        <f t="shared" ref="I57:M57" si="15">ABS((I10-I33)/I10)</f>
+        <v>2.3255813953488292E-2</v>
+      </c>
+      <c r="J57" s="14">
+        <f t="shared" si="15"/>
+        <v>2.7777777777777801E-2</v>
+      </c>
+      <c r="K57" s="14">
+        <f t="shared" si="15"/>
+        <v>9.0909090909090995E-2</v>
+      </c>
+      <c r="L57" s="14">
+        <f t="shared" si="15"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="M57" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="14">
+        <f t="shared" ref="B58:F58" si="16">ABS((B11-B34)/B11)</f>
+        <v>8.4552845528455337E-2</v>
+      </c>
+      <c r="C58" s="14">
+        <f t="shared" si="16"/>
+        <v>8.6991869918699088E-2</v>
+      </c>
+      <c r="D58" s="14">
+        <f t="shared" si="16"/>
+        <v>0.10082644628099165</v>
+      </c>
+      <c r="E58" s="14">
+        <f t="shared" si="16"/>
+        <v>9.8360655737704916E-2</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I58" s="14">
+        <f t="shared" ref="I58:M58" si="17">ABS((I11-I34)/I11)</f>
+        <v>8.4552845528455337E-2</v>
+      </c>
+      <c r="J58" s="14">
+        <f t="shared" si="17"/>
+        <v>0.10833333333333334</v>
+      </c>
+      <c r="K58" s="14">
+        <f t="shared" si="17"/>
+        <v>0.10840336134453786</v>
+      </c>
+      <c r="L58" s="14">
+        <f t="shared" si="17"/>
+        <v>0.14999999999999994</v>
+      </c>
+      <c r="M58" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="14">
+        <f t="shared" ref="B59:F59" si="18">ABS((B12-B35)/B12)</f>
+        <v>2.3391812865496991E-2</v>
+      </c>
+      <c r="C59" s="14">
+        <f t="shared" si="18"/>
+        <v>2.8901734104046242E-2</v>
+      </c>
+      <c r="D59" s="14">
+        <f t="shared" si="18"/>
+        <v>4.6511627906976785E-2</v>
+      </c>
+      <c r="E59" s="14">
+        <f t="shared" si="18"/>
+        <v>7.9999999999999918E-2</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I59" s="14">
+        <f t="shared" ref="I59:M59" si="19">ABS((I12-I35)/I12)</f>
+        <v>2.3391812865496991E-2</v>
+      </c>
+      <c r="J59" s="14">
+        <f t="shared" si="19"/>
+        <v>4.7058823529411806E-2</v>
+      </c>
+      <c r="K59" s="14">
+        <f t="shared" si="19"/>
+        <v>5.9171597633136098E-2</v>
+      </c>
+      <c r="L59" s="14">
+        <f t="shared" si="19"/>
+        <v>0.12121212121212122</v>
+      </c>
+      <c r="M59" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="14">
+        <f t="shared" ref="B60:F60" si="20">ABS((B13-B36)/B13)</f>
+        <v>4.0404040404040435E-2</v>
+      </c>
+      <c r="C60" s="14">
+        <f t="shared" si="20"/>
+        <v>6.3157894736842066E-2</v>
+      </c>
+      <c r="D60" s="14">
+        <f t="shared" si="20"/>
+        <v>0.1022727272727271</v>
+      </c>
+      <c r="E60" s="14">
+        <f t="shared" si="20"/>
+        <v>0.21052631578947364</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I60" s="14">
+        <f t="shared" ref="I60:M60" si="21">ABS((I13-I36)/I13)</f>
+        <v>4.0404040404040435E-2</v>
+      </c>
+      <c r="J60" s="14">
+        <f t="shared" si="21"/>
+        <v>7.4468085106382906E-2</v>
+      </c>
+      <c r="K60" s="14">
+        <f t="shared" si="21"/>
+        <v>0.1022727272727271</v>
+      </c>
+      <c r="L60" s="14">
+        <f t="shared" si="21"/>
+        <v>0.2400000000000001</v>
+      </c>
+      <c r="M60" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="14">
+        <f t="shared" ref="B61:F61" si="22">ABS((B14-B37)/B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C61" s="14">
+        <f t="shared" si="22"/>
+        <v>4.5454545454545491E-2</v>
+      </c>
+      <c r="D61" s="14">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="E61" s="14">
+        <f t="shared" si="22"/>
+        <v>5.2631578947368356E-2</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="14">
+        <f t="shared" ref="I61:M61" si="23">ABS((I14-I37)/I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="14">
+        <f t="shared" si="23"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="K61" s="14">
+        <f t="shared" si="23"/>
+        <v>4.3478260869565258E-2</v>
+      </c>
+      <c r="L61" s="14">
+        <f t="shared" si="23"/>
+        <v>6.4516129032257979E-2</v>
+      </c>
+      <c r="M61" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="14">
+        <f t="shared" ref="B62:F62" si="24">ABS((B15-B38)/B15)</f>
+        <v>1.5384615384615398E-2</v>
+      </c>
+      <c r="C62" s="14">
+        <f t="shared" si="24"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D62" s="14">
+        <f t="shared" si="24"/>
+        <v>1.7391304347826105E-2</v>
+      </c>
+      <c r="E62" s="14">
+        <f t="shared" si="24"/>
+        <v>3.235294117647055E-2</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="14">
+        <f t="shared" ref="I62:M62" si="25">ABS((I15-I38)/I15)</f>
+        <v>1.5384615384615398E-2</v>
+      </c>
+      <c r="J62" s="14">
+        <f t="shared" si="25"/>
+        <v>4.999999999999992E-2</v>
+      </c>
+      <c r="K62" s="14">
+        <f t="shared" si="25"/>
+        <v>5.714285714285719E-2</v>
+      </c>
+      <c r="L62" s="14">
+        <f t="shared" si="25"/>
+        <v>7.1428571428571494E-2</v>
+      </c>
+      <c r="M62" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="14">
+        <f t="shared" ref="B63:F63" si="26">ABS((B16-B39)/B16)</f>
+        <v>3.6000000000000032E-2</v>
+      </c>
+      <c r="C63" s="14">
+        <f t="shared" si="26"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="D63" s="14">
+        <f t="shared" si="26"/>
+        <v>4.1666666666666709E-3</v>
+      </c>
+      <c r="E63" s="14">
+        <f t="shared" si="26"/>
+        <v>3.7142857142857019E-2</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" s="14">
+        <f t="shared" ref="I63:M63" si="27">ABS((I16-I39)/I16)</f>
+        <v>3.6000000000000032E-2</v>
+      </c>
+      <c r="J63" s="14">
+        <f t="shared" si="27"/>
+        <v>1.0526315789473693E-2</v>
+      </c>
+      <c r="K63" s="14">
+        <f t="shared" si="27"/>
+        <v>3.181818181818185E-2</v>
+      </c>
+      <c r="L63" s="14">
+        <f t="shared" si="27"/>
+        <v>6.2068965517241441E-2</v>
+      </c>
+      <c r="M63" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="90.75" thickBot="1">
+      <c r="A64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="14">
+        <f t="shared" ref="B64:F64" si="28">ABS((B17-B40)/B17)</f>
+        <v>5.5263157894736889E-2</v>
+      </c>
+      <c r="C64" s="14">
+        <f t="shared" si="28"/>
+        <v>4.7058823529411806E-2</v>
+      </c>
+      <c r="D64" s="14">
+        <f t="shared" si="28"/>
+        <v>1.0526315789473693E-2</v>
+      </c>
+      <c r="E64" s="14">
+        <f t="shared" si="28"/>
+        <v>2.6923076923076945E-2</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" s="14">
+        <f t="shared" ref="I64:M64" si="29">ABS((I17-I40)/I17)</f>
+        <v>5.5263157894736889E-2</v>
+      </c>
+      <c r="J64" s="14">
+        <f t="shared" si="29"/>
+        <v>5.3333333333333385E-2</v>
+      </c>
+      <c r="K64" s="14">
+        <f t="shared" si="29"/>
+        <v>1.6666666666666684E-2</v>
+      </c>
+      <c r="L64" s="14">
+        <f t="shared" si="29"/>
+        <v>6.8181818181818121E-2</v>
+      </c>
+      <c r="M64" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="14">
+        <f t="shared" ref="B65:F65" si="30">ABS((B18-B41)/B18)</f>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="C65" s="14">
+        <f t="shared" si="30"/>
+        <v>5.4054054054053918E-2</v>
+      </c>
+      <c r="D65" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E65" s="14">
+        <f t="shared" si="30"/>
+        <v>7.6923076923076844E-2</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="14">
+        <f t="shared" ref="I65:M65" si="31">ABS((I18-I41)/I18)</f>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="J65" s="14">
+        <f t="shared" si="31"/>
+        <v>6.2500000000000056E-2</v>
+      </c>
+      <c r="K65" s="14">
+        <f t="shared" si="31"/>
+        <v>9.9999999999999908E-2</v>
+      </c>
+      <c r="L65" s="14">
+        <f t="shared" si="31"/>
+        <v>8.9552238805970019E-2</v>
+      </c>
+      <c r="M65" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="14">
+        <f t="shared" ref="B66:F66" si="32">ABS((B19-B42)/B19)</f>
+        <v>4.0175557056043212E-2</v>
+      </c>
+      <c r="C66" s="14">
+        <f t="shared" si="32"/>
+        <v>4.6475625823451883E-2</v>
+      </c>
+      <c r="D66" s="14">
+        <f t="shared" si="32"/>
+        <v>6.6965716116629284E-2</v>
+      </c>
+      <c r="E66" s="14">
+        <f t="shared" si="32"/>
+        <v>0.15680922050348803</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" s="14">
+        <f t="shared" ref="I66:M66" si="33">ABS((I19-I42)/I19)</f>
+        <v>4.0175557056043212E-2</v>
+      </c>
+      <c r="J66" s="14">
+        <f t="shared" si="33"/>
+        <v>4.5753785385121794E-2</v>
+      </c>
+      <c r="K66" s="14">
+        <f t="shared" si="33"/>
+        <v>6.3557968700095821E-2</v>
+      </c>
+      <c r="L66" s="14">
+        <f t="shared" si="33"/>
+        <v>0.15957130098243524</v>
+      </c>
+      <c r="M66" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="30.75" thickBot="1">
+      <c r="A67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="14">
+        <f t="shared" ref="B67:F67" si="34">ABS((B20-B43)/B20)</f>
+        <v>0.14062499999999992</v>
+      </c>
+      <c r="C67" s="14">
+        <f t="shared" si="34"/>
+        <v>0.12592592592592589</v>
+      </c>
+      <c r="D67" s="14">
+        <f t="shared" si="34"/>
+        <v>0.12000000000000005</v>
+      </c>
+      <c r="E67" s="14">
+        <f t="shared" si="34"/>
+        <v>0.19576719576719592</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I67" s="14">
+        <f t="shared" ref="I67:M67" si="35">ABS((I20-I43)/I20)</f>
+        <v>0.14062499999999992</v>
+      </c>
+      <c r="J67" s="14">
+        <f t="shared" si="35"/>
+        <v>0.12592592592592589</v>
+      </c>
+      <c r="K67" s="14">
+        <f t="shared" si="35"/>
+        <v>0.11258278145695372</v>
+      </c>
+      <c r="L67" s="14">
+        <f t="shared" si="35"/>
+        <v>0.17587939698492464</v>
+      </c>
+      <c r="M67" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="30.75" thickBot="1">
+      <c r="A68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M68" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="4">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="K24:M24"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
+  <conditionalFormatting sqref="B50:F68">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50:M68">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>